<commit_message>
adding web service changes
</commit_message>
<xml_diff>
--- a/public/assets/uploads/Uploads/company_current_stock/companycurrentstock_data.xlsx
+++ b/public/assets/uploads/Uploads/company_current_stock/companycurrentstock_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Product SKU Code</t>
   </si>
@@ -50,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -108,7 +108,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,7 +460,7 @@
         <v>200</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>1009</v>
       </c>
       <c r="F2" s="3">
         <v>43252</v>
@@ -476,9 +476,6 @@
       <c r="A3">
         <v>58515696</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
       <c r="C3" s="1">
         <v>2222</v>
       </c>
@@ -486,7 +483,7 @@
         <v>300</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>509</v>
       </c>
       <c r="F3" s="3">
         <v>43253</v>
@@ -508,14 +505,11 @@
       <c r="C4" s="1">
         <v>33333</v>
       </c>
-      <c r="D4">
-        <v>400</v>
-      </c>
       <c r="E4">
-        <v>150</v>
+        <v>1059</v>
       </c>
       <c r="F4" s="3">
-        <v>43254</v>
+        <v>43259</v>
       </c>
       <c r="G4" s="3">
         <v>42522</v>
@@ -536,7 +530,7 @@
         <v>500</v>
       </c>
       <c r="E5">
-        <v>160</v>
+        <v>1609</v>
       </c>
       <c r="F5" s="3">
         <v>43256</v>

</xml_diff>